<commit_message>
Even Final report newly done
</commit_message>
<xml_diff>
--- a/Qualität_11_24.xlsx
+++ b/Qualität_11_24.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Zeilenbeschriftungen</t>
   </si>
@@ -72,21 +72,6 @@
     <t>1002000/555555/Pan les</t>
   </si>
   <si>
-    <t>1002000/6666/Pan yes</t>
-  </si>
-  <si>
-    <t>1003000/777/Pan hes</t>
-  </si>
-  <si>
-    <t>1003000/222/Pan kes</t>
-  </si>
-  <si>
-    <t>1003000/33/pan qes</t>
-  </si>
-  <si>
-    <t>1003000/18/pan bes</t>
-  </si>
-  <si>
     <t>Gesamtergebnis</t>
   </si>
   <si>
@@ -105,7 +90,7 @@
     <t>Qualität Intern:</t>
   </si>
   <si>
-    <t>Echt</t>
+    <t>Echt:</t>
   </si>
 </sst>
 </file>
@@ -445,11 +430,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1047"/>
+  <dimension ref="A1:O1043"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1031" workbookViewId="0">
-      <selection activeCell="C1018" sqref="C1018"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -507,11 +490,11 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:N8" si="0">SUM(B2:M2)</f>
+        <f>SUM(B2:M2)</f>
         <v>1</v>
       </c>
       <c r="O2">
@@ -522,281 +505,203 @@
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="N3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>SUM(B3:M3)</f>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="1003" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1003" t="s">
         <v>17</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="N4">
+      <c r="B1003">
+        <f t="shared" ref="B1003:M1003" si="0">SUM(B2:B3)</f>
+        <v>0</v>
+      </c>
+      <c r="C1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J1003">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="K1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M1003">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1014" t="s">
         <v>18</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C1014">
+        <f>COUNT(B2:M1003)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1017" t="s">
         <v>19</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="O6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1007" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1007" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1007">
-        <f t="shared" ref="B1007:M1007" si="1">SUM(B2:B7)</f>
-        <v>0</v>
-      </c>
-      <c r="C1007">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D1007">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E1007">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F1007">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G1007">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H1007">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I1007">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="J1007">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="K1007">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L1007">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M1007">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="B1017" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="1018" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1018" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1018">
-        <f>COUNT(B2:M1007)</f>
-        <v>23</v>
+      <c r="B1018">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1019">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1020">
+        <v>19</v>
       </c>
     </row>
     <row r="1021" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1021" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1021" t="s">
-        <v>14</v>
+      <c r="B1021">
+        <v>25</v>
       </c>
     </row>
     <row r="1022" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1022">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1023" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1023">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="1024" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1024">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1025">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1026">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1027">
-        <v>27</v>
+      <c r="B1027" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1028">
-        <v>30</v>
+      <c r="A1028" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1029">
-        <v>31</v>
+      <c r="A1029" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1030">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="1031" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1031" t="s">
+      <c r="B1031">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1032">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1033">
         <v>25</v>
-      </c>
-    </row>
-    <row r="1032" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1032" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="1033" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1033" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1033" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="1034" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1034">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1035">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1036">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1037">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="1038" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1038">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1039" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1039">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="1040" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1040">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="1041" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1041">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="1042" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1042">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1043" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1043" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="1047" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1047" t="s">
-        <v>28</v>
+      <c r="B1039" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1043" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Newly done, more of classes used
</commit_message>
<xml_diff>
--- a/Qualität_11_24.xlsx
+++ b/Qualität_11_24.xlsx
@@ -507,16 +507,10 @@
           <t>1002000/44444/Pan pes</t>
         </is>
       </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
       <c r="N2">
         <f>SUM(B2:M2)</f>
         <v/>
       </c>
-      <c r="O2" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -524,15 +518,9 @@
           <t>1002000/555555/Pan les</t>
         </is>
       </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
       <c r="N3">
         <f>SUM(B3:M3)</f>
         <v/>
-      </c>
-      <c r="O3" t="n">
-        <v>30</v>
       </c>
     </row>
     <row r="1003">

</xml_diff>

<commit_message>
My god... excel end of report working??!
</commit_message>
<xml_diff>
--- a/Qualität_11_24.xlsx
+++ b/Qualität_11_24.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -232,13 +232,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -271,11 +276,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -580,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1066"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1038" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -670,554 +677,1470 @@
         <v>30</v>
       </c>
     </row>
-    <row r="1003" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1003" t="s">
+    <row r="1003" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1003" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1003">
+      <c r="B1003" s="1">
         <f t="shared" ref="B1003:M1003" si="0">SUM(B2:B3)</f>
         <v>0</v>
       </c>
-      <c r="C1003">
+      <c r="C1003" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D1003">
+      <c r="D1003" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E1003">
+      <c r="E1003" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F1003">
+      <c r="F1003" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G1003">
+      <c r="G1003" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H1003">
+      <c r="H1003" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I1003">
+      <c r="I1003" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J1003">
+      <c r="J1003" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K1003">
+      <c r="K1003" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L1003">
+      <c r="L1003" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M1003">
+      <c r="M1003" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="1014" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1014" t="s">
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="1"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="1"/>
+      <c r="G1005" s="1"/>
+      <c r="H1005" s="1"/>
+      <c r="I1005" s="1"/>
+      <c r="J1005" s="1"/>
+      <c r="K1005" s="1"/>
+      <c r="L1005" s="1"/>
+      <c r="M1005" s="1"/>
+      <c r="N1005" s="1"/>
+      <c r="O1005" s="1"/>
+      <c r="P1005" s="1"/>
+      <c r="Q1005" s="1"/>
+      <c r="R1005" s="1"/>
+    </row>
+    <row r="1006" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="1"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="1"/>
+      <c r="G1006" s="1"/>
+      <c r="H1006" s="1"/>
+      <c r="I1006" s="1"/>
+      <c r="J1006" s="1"/>
+      <c r="K1006" s="1"/>
+      <c r="L1006" s="1"/>
+      <c r="M1006" s="1"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+    </row>
+    <row r="1007" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="1"/>
+      <c r="E1007" s="1"/>
+      <c r="F1007" s="1"/>
+      <c r="G1007" s="1"/>
+      <c r="H1007" s="1"/>
+      <c r="I1007" s="1"/>
+      <c r="J1007" s="1"/>
+      <c r="K1007" s="1"/>
+      <c r="L1007" s="1"/>
+      <c r="M1007" s="1"/>
+      <c r="N1007" s="1"/>
+      <c r="O1007" s="1"/>
+      <c r="P1007" s="1"/>
+      <c r="Q1007" s="1"/>
+      <c r="R1007" s="1"/>
+    </row>
+    <row r="1008" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="1"/>
+      <c r="E1008" s="1"/>
+      <c r="F1008" s="1"/>
+      <c r="G1008" s="1"/>
+      <c r="H1008" s="1"/>
+      <c r="I1008" s="1"/>
+      <c r="J1008" s="1"/>
+      <c r="K1008" s="1"/>
+      <c r="L1008" s="1"/>
+      <c r="M1008" s="1"/>
+      <c r="N1008" s="1"/>
+      <c r="O1008" s="1"/>
+      <c r="P1008" s="1"/>
+      <c r="Q1008" s="1"/>
+      <c r="R1008" s="1"/>
+    </row>
+    <row r="1009" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+      <c r="D1009" s="1"/>
+      <c r="E1009" s="1"/>
+      <c r="F1009" s="1"/>
+      <c r="G1009" s="1"/>
+      <c r="H1009" s="1"/>
+      <c r="I1009" s="1"/>
+      <c r="J1009" s="1"/>
+      <c r="K1009" s="1"/>
+      <c r="L1009" s="1"/>
+      <c r="M1009" s="1"/>
+      <c r="N1009" s="1"/>
+      <c r="O1009" s="1"/>
+      <c r="P1009" s="1"/>
+      <c r="Q1009" s="1"/>
+      <c r="R1009" s="1"/>
+    </row>
+    <row r="1010" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="1"/>
+      <c r="C1010" s="1"/>
+      <c r="D1010" s="1"/>
+      <c r="E1010" s="1"/>
+      <c r="F1010" s="1"/>
+      <c r="G1010" s="1"/>
+      <c r="H1010" s="1"/>
+      <c r="I1010" s="1"/>
+      <c r="J1010" s="1"/>
+      <c r="K1010" s="1"/>
+      <c r="L1010" s="1"/>
+      <c r="M1010" s="1"/>
+      <c r="N1010" s="1"/>
+      <c r="O1010" s="1"/>
+      <c r="P1010" s="1"/>
+      <c r="Q1010" s="1"/>
+      <c r="R1010" s="1"/>
+    </row>
+    <row r="1011" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1011" s="1"/>
+      <c r="B1011" s="1"/>
+      <c r="C1011" s="1"/>
+      <c r="D1011" s="1"/>
+      <c r="E1011" s="1"/>
+      <c r="F1011" s="1"/>
+      <c r="G1011" s="1"/>
+      <c r="H1011" s="1"/>
+      <c r="I1011" s="1"/>
+      <c r="J1011" s="1"/>
+      <c r="K1011" s="1"/>
+      <c r="L1011" s="1"/>
+      <c r="M1011" s="1"/>
+      <c r="N1011" s="1"/>
+      <c r="O1011" s="1"/>
+      <c r="P1011" s="1"/>
+      <c r="Q1011" s="1"/>
+      <c r="R1011" s="1"/>
+    </row>
+    <row r="1012" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1012" s="1"/>
+      <c r="B1012" s="1"/>
+      <c r="C1012" s="1"/>
+      <c r="D1012" s="1"/>
+      <c r="E1012" s="1"/>
+      <c r="F1012" s="1"/>
+      <c r="G1012" s="1"/>
+      <c r="H1012" s="1"/>
+      <c r="I1012" s="1"/>
+      <c r="J1012" s="1"/>
+      <c r="K1012" s="1"/>
+      <c r="L1012" s="1"/>
+      <c r="M1012" s="1"/>
+      <c r="N1012" s="1"/>
+      <c r="O1012" s="1"/>
+      <c r="P1012" s="1"/>
+      <c r="Q1012" s="1"/>
+      <c r="R1012" s="1"/>
+    </row>
+    <row r="1013" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1013" s="1"/>
+      <c r="B1013" s="1"/>
+      <c r="C1013" s="1"/>
+      <c r="D1013" s="1"/>
+      <c r="E1013" s="1"/>
+      <c r="F1013" s="1"/>
+      <c r="G1013" s="1"/>
+      <c r="H1013" s="1"/>
+      <c r="I1013" s="1"/>
+      <c r="J1013" s="1"/>
+      <c r="K1013" s="1"/>
+      <c r="L1013" s="1"/>
+      <c r="M1013" s="1"/>
+      <c r="N1013" s="1"/>
+      <c r="O1013" s="1"/>
+      <c r="P1013" s="1"/>
+      <c r="Q1013" s="1"/>
+      <c r="R1013" s="1"/>
+    </row>
+    <row r="1014" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1014" s="1"/>
+      <c r="B1014" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1014">
+      <c r="C1014" s="1">
         <f>COUNT(B2:M1003)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="1017" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1017" t="s">
+      <c r="D1014" s="1"/>
+      <c r="E1014" s="1"/>
+      <c r="F1014" s="1"/>
+      <c r="G1014" s="1"/>
+      <c r="H1014" s="1"/>
+      <c r="I1014" s="1"/>
+      <c r="J1014" s="1"/>
+      <c r="K1014" s="1"/>
+      <c r="L1014" s="1"/>
+      <c r="M1014" s="1"/>
+      <c r="N1014" s="1"/>
+      <c r="O1014" s="1"/>
+      <c r="P1014" s="1"/>
+      <c r="Q1014" s="1"/>
+      <c r="R1014" s="1"/>
+    </row>
+    <row r="1015" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1015" s="1"/>
+      <c r="B1015" s="1"/>
+      <c r="C1015" s="1"/>
+      <c r="D1015" s="1"/>
+      <c r="E1015" s="1"/>
+      <c r="F1015" s="1"/>
+      <c r="G1015" s="1"/>
+      <c r="H1015" s="1"/>
+      <c r="I1015" s="1"/>
+      <c r="J1015" s="1"/>
+      <c r="K1015" s="1"/>
+      <c r="L1015" s="1"/>
+      <c r="M1015" s="1"/>
+      <c r="N1015" s="1"/>
+      <c r="O1015" s="1"/>
+      <c r="P1015" s="1"/>
+      <c r="Q1015" s="1"/>
+      <c r="R1015" s="1"/>
+    </row>
+    <row r="1016" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1016" s="1"/>
+      <c r="B1016" s="1"/>
+      <c r="C1016" s="1"/>
+      <c r="D1016" s="1"/>
+      <c r="E1016" s="1"/>
+      <c r="F1016" s="1"/>
+      <c r="G1016" s="1"/>
+      <c r="H1016" s="1"/>
+      <c r="I1016" s="1"/>
+      <c r="J1016" s="1"/>
+      <c r="K1016" s="1"/>
+      <c r="L1016" s="1"/>
+      <c r="M1016" s="1"/>
+      <c r="N1016" s="1"/>
+      <c r="O1016" s="1"/>
+      <c r="P1016" s="1"/>
+      <c r="Q1016" s="1"/>
+      <c r="R1016" s="1"/>
+    </row>
+    <row r="1017" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1017" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1017" t="s">
+      <c r="B1017" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1018" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1018">
+      <c r="C1017" s="1"/>
+      <c r="D1017" s="1"/>
+      <c r="E1017" s="1"/>
+      <c r="F1017" s="1"/>
+      <c r="G1017" s="1"/>
+      <c r="H1017" s="1"/>
+      <c r="I1017" s="1"/>
+      <c r="J1017" s="1"/>
+      <c r="K1017" s="1"/>
+      <c r="L1017" s="1"/>
+      <c r="M1017" s="1"/>
+      <c r="N1017" s="1"/>
+      <c r="O1017" s="1"/>
+      <c r="P1017" s="1"/>
+      <c r="Q1017" s="1"/>
+      <c r="R1017" s="1"/>
+    </row>
+    <row r="1018" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1018" s="1"/>
+      <c r="B1018" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="1019" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1019">
+      <c r="C1018" s="1"/>
+      <c r="D1018" s="1"/>
+      <c r="E1018" s="1"/>
+      <c r="F1018" s="1"/>
+      <c r="G1018" s="1"/>
+      <c r="H1018" s="1"/>
+      <c r="I1018" s="1"/>
+      <c r="J1018" s="1"/>
+      <c r="K1018" s="1"/>
+      <c r="L1018" s="1"/>
+      <c r="M1018" s="1"/>
+      <c r="N1018" s="1"/>
+      <c r="O1018" s="1"/>
+      <c r="P1018" s="1"/>
+      <c r="Q1018" s="1"/>
+      <c r="R1018" s="1"/>
+    </row>
+    <row r="1019" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1019" s="1"/>
+      <c r="B1019" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="1020" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1020">
+      <c r="C1019" s="1"/>
+      <c r="D1019" s="1"/>
+      <c r="E1019" s="1"/>
+      <c r="F1019" s="1"/>
+      <c r="G1019" s="1"/>
+      <c r="H1019" s="1"/>
+      <c r="I1019" s="1"/>
+      <c r="J1019" s="1"/>
+      <c r="K1019" s="1"/>
+      <c r="L1019" s="1"/>
+      <c r="M1019" s="1"/>
+      <c r="N1019" s="1"/>
+      <c r="O1019" s="1"/>
+      <c r="P1019" s="1"/>
+      <c r="Q1019" s="1"/>
+      <c r="R1019" s="1"/>
+    </row>
+    <row r="1020" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1020" s="1"/>
+      <c r="B1020" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="1021" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1021">
+      <c r="C1020" s="1"/>
+      <c r="D1020" s="1"/>
+      <c r="E1020" s="1"/>
+      <c r="F1020" s="1"/>
+      <c r="G1020" s="1"/>
+      <c r="H1020" s="1"/>
+      <c r="I1020" s="1"/>
+      <c r="J1020" s="1"/>
+      <c r="K1020" s="1"/>
+      <c r="L1020" s="1"/>
+      <c r="M1020" s="1"/>
+      <c r="N1020" s="1"/>
+      <c r="O1020" s="1"/>
+      <c r="P1020" s="1"/>
+      <c r="Q1020" s="1"/>
+      <c r="R1020" s="1"/>
+    </row>
+    <row r="1021" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1021" s="1"/>
+      <c r="B1021" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="1022" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1022">
+      <c r="C1021" s="1"/>
+      <c r="D1021" s="1"/>
+      <c r="E1021" s="1"/>
+      <c r="F1021" s="1"/>
+      <c r="G1021" s="1"/>
+      <c r="H1021" s="1"/>
+      <c r="I1021" s="1"/>
+      <c r="J1021" s="1"/>
+      <c r="K1021" s="1"/>
+      <c r="L1021" s="1"/>
+      <c r="M1021" s="1"/>
+      <c r="N1021" s="1"/>
+      <c r="O1021" s="1"/>
+      <c r="P1021" s="1"/>
+      <c r="Q1021" s="1"/>
+      <c r="R1021" s="1"/>
+    </row>
+    <row r="1022" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1022" s="1"/>
+      <c r="B1022" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="1023" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1023">
+      <c r="C1022" s="1"/>
+      <c r="D1022" s="1"/>
+      <c r="E1022" s="1"/>
+      <c r="F1022" s="1"/>
+      <c r="G1022" s="1"/>
+      <c r="H1022" s="1"/>
+      <c r="I1022" s="1"/>
+      <c r="J1022" s="1"/>
+      <c r="K1022" s="1"/>
+      <c r="L1022" s="1"/>
+      <c r="M1022" s="1"/>
+      <c r="N1022" s="1"/>
+      <c r="O1022" s="1"/>
+      <c r="P1022" s="1"/>
+      <c r="Q1022" s="1"/>
+      <c r="R1022" s="1"/>
+    </row>
+    <row r="1023" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1023" s="1"/>
+      <c r="B1023" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="1024" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1024">
+      <c r="C1023" s="1"/>
+      <c r="D1023" s="1"/>
+      <c r="E1023" s="1"/>
+      <c r="F1023" s="1"/>
+      <c r="G1023" s="1"/>
+      <c r="H1023" s="1"/>
+      <c r="I1023" s="1"/>
+      <c r="J1023" s="1"/>
+      <c r="K1023" s="1"/>
+      <c r="L1023" s="1"/>
+      <c r="M1023" s="1"/>
+      <c r="N1023" s="1"/>
+      <c r="O1023" s="1"/>
+      <c r="P1023" s="1"/>
+      <c r="Q1023" s="1"/>
+      <c r="R1023" s="1"/>
+    </row>
+    <row r="1024" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="1025" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1025">
+      <c r="C1024" s="1"/>
+      <c r="D1024" s="1"/>
+      <c r="E1024" s="1"/>
+      <c r="F1024" s="1"/>
+      <c r="G1024" s="1"/>
+      <c r="H1024" s="1"/>
+      <c r="I1024" s="1"/>
+      <c r="J1024" s="1"/>
+      <c r="K1024" s="1"/>
+      <c r="L1024" s="1"/>
+      <c r="M1024" s="1"/>
+      <c r="N1024" s="1"/>
+      <c r="O1024" s="1"/>
+      <c r="P1024" s="1"/>
+      <c r="Q1024" s="1"/>
+      <c r="R1024" s="1"/>
+    </row>
+    <row r="1025" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="1026" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1026">
+      <c r="C1025" s="1"/>
+      <c r="D1025" s="1"/>
+      <c r="E1025" s="1"/>
+      <c r="F1025" s="1"/>
+      <c r="G1025" s="1"/>
+      <c r="H1025" s="1"/>
+      <c r="I1025" s="1"/>
+      <c r="J1025" s="1"/>
+      <c r="K1025" s="1"/>
+      <c r="L1025" s="1"/>
+      <c r="M1025" s="1"/>
+      <c r="N1025" s="1"/>
+      <c r="O1025" s="1"/>
+      <c r="P1025" s="1"/>
+      <c r="Q1025" s="1"/>
+      <c r="R1025" s="1"/>
+    </row>
+    <row r="1026" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1026" s="1"/>
+      <c r="B1026" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="1027" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1027" t="s">
+      <c r="C1026" s="1"/>
+      <c r="D1026" s="1"/>
+      <c r="E1026" s="1"/>
+      <c r="F1026" s="1"/>
+      <c r="G1026" s="1"/>
+      <c r="H1026" s="1"/>
+      <c r="I1026" s="1"/>
+      <c r="J1026" s="1"/>
+      <c r="K1026" s="1"/>
+      <c r="L1026" s="1"/>
+      <c r="M1026" s="1"/>
+      <c r="N1026" s="1"/>
+      <c r="O1026" s="1"/>
+      <c r="P1026" s="1"/>
+      <c r="Q1026" s="1"/>
+      <c r="R1026" s="1"/>
+    </row>
+    <row r="1027" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1027" s="1"/>
+      <c r="B1027" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="1028" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1028" t="s">
+      <c r="C1027" s="1"/>
+      <c r="D1027" s="1"/>
+      <c r="E1027" s="1"/>
+      <c r="F1027" s="1"/>
+      <c r="G1027" s="1"/>
+      <c r="H1027" s="1"/>
+      <c r="I1027" s="1"/>
+      <c r="J1027" s="1"/>
+      <c r="K1027" s="1"/>
+      <c r="L1027" s="1"/>
+      <c r="M1027" s="1"/>
+      <c r="N1027" s="1"/>
+      <c r="O1027" s="1"/>
+      <c r="P1027" s="1"/>
+      <c r="Q1027" s="1"/>
+      <c r="R1027" s="1"/>
+    </row>
+    <row r="1028" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1028" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="1029" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1029" t="s">
+      <c r="B1028" s="1"/>
+      <c r="C1028" s="1"/>
+      <c r="D1028" s="1"/>
+      <c r="E1028" s="1"/>
+      <c r="F1028" s="1"/>
+      <c r="G1028" s="1"/>
+      <c r="H1028" s="1"/>
+      <c r="I1028" s="1"/>
+      <c r="J1028" s="1"/>
+      <c r="K1028" s="1"/>
+      <c r="L1028" s="1"/>
+      <c r="M1028" s="1"/>
+      <c r="N1028" s="1"/>
+      <c r="O1028" s="1"/>
+      <c r="P1028" s="1"/>
+      <c r="Q1028" s="1"/>
+      <c r="R1028" s="1"/>
+    </row>
+    <row r="1029" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1029" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1029" t="s">
+      <c r="B1029" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="1030" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1030">
+      <c r="C1029" s="1"/>
+      <c r="D1029" s="1"/>
+      <c r="E1029" s="1"/>
+      <c r="F1029" s="1"/>
+      <c r="G1029" s="1"/>
+      <c r="H1029" s="1"/>
+      <c r="I1029" s="1"/>
+      <c r="J1029" s="1"/>
+      <c r="K1029" s="1"/>
+      <c r="L1029" s="1"/>
+      <c r="M1029" s="1"/>
+      <c r="N1029" s="1"/>
+      <c r="O1029" s="1"/>
+      <c r="P1029" s="1"/>
+      <c r="Q1029" s="1"/>
+      <c r="R1029" s="1"/>
+    </row>
+    <row r="1030" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1030" s="1"/>
+      <c r="B1030" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="1031" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1031">
+      <c r="C1030" s="1"/>
+      <c r="D1030" s="1"/>
+      <c r="E1030" s="1"/>
+      <c r="F1030" s="1"/>
+      <c r="G1030" s="1"/>
+      <c r="H1030" s="1"/>
+      <c r="I1030" s="1"/>
+      <c r="J1030" s="1"/>
+      <c r="K1030" s="1"/>
+      <c r="L1030" s="1"/>
+      <c r="M1030" s="1"/>
+      <c r="N1030" s="1"/>
+      <c r="O1030" s="1"/>
+      <c r="P1030" s="1"/>
+      <c r="Q1030" s="1"/>
+      <c r="R1030" s="1"/>
+    </row>
+    <row r="1031" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1031" s="1"/>
+      <c r="B1031" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="1032" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1032">
+      <c r="C1031" s="1"/>
+      <c r="D1031" s="1"/>
+      <c r="E1031" s="1"/>
+      <c r="F1031" s="1"/>
+      <c r="G1031" s="1"/>
+      <c r="H1031" s="1"/>
+      <c r="I1031" s="1"/>
+      <c r="J1031" s="1"/>
+      <c r="K1031" s="1"/>
+      <c r="L1031" s="1"/>
+      <c r="M1031" s="1"/>
+      <c r="N1031" s="1"/>
+      <c r="O1031" s="1"/>
+      <c r="P1031" s="1"/>
+      <c r="Q1031" s="1"/>
+      <c r="R1031" s="1"/>
+    </row>
+    <row r="1032" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1032" s="1"/>
+      <c r="B1032" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="1033" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1033">
+      <c r="C1032" s="1"/>
+      <c r="D1032" s="1"/>
+      <c r="E1032" s="1"/>
+      <c r="F1032" s="1"/>
+      <c r="G1032" s="1"/>
+      <c r="H1032" s="1"/>
+      <c r="I1032" s="1"/>
+      <c r="J1032" s="1"/>
+      <c r="K1032" s="1"/>
+      <c r="L1032" s="1"/>
+      <c r="M1032" s="1"/>
+      <c r="N1032" s="1"/>
+      <c r="O1032" s="1"/>
+      <c r="P1032" s="1"/>
+      <c r="Q1032" s="1"/>
+      <c r="R1032" s="1"/>
+    </row>
+    <row r="1033" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1033" s="1"/>
+      <c r="B1033" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="1034" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1034">
+      <c r="C1033" s="1"/>
+      <c r="D1033" s="1"/>
+      <c r="E1033" s="1"/>
+      <c r="F1033" s="1"/>
+      <c r="G1033" s="1"/>
+      <c r="H1033" s="1"/>
+      <c r="I1033" s="1"/>
+      <c r="J1033" s="1"/>
+      <c r="K1033" s="1"/>
+      <c r="L1033" s="1"/>
+      <c r="M1033" s="1"/>
+      <c r="N1033" s="1"/>
+      <c r="O1033" s="1"/>
+      <c r="P1033" s="1"/>
+      <c r="Q1033" s="1"/>
+      <c r="R1033" s="1"/>
+    </row>
+    <row r="1034" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1034" s="1"/>
+      <c r="B1034" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="1035" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1035">
+      <c r="C1034" s="1"/>
+      <c r="D1034" s="1"/>
+      <c r="E1034" s="1"/>
+      <c r="F1034" s="1"/>
+      <c r="G1034" s="1"/>
+      <c r="H1034" s="1"/>
+      <c r="I1034" s="1"/>
+      <c r="J1034" s="1"/>
+      <c r="K1034" s="1"/>
+      <c r="L1034" s="1"/>
+      <c r="M1034" s="1"/>
+      <c r="N1034" s="1"/>
+      <c r="O1034" s="1"/>
+      <c r="P1034" s="1"/>
+      <c r="Q1034" s="1"/>
+      <c r="R1034" s="1"/>
+    </row>
+    <row r="1035" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1035" s="1"/>
+      <c r="B1035" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="1036" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1036">
+      <c r="C1035" s="1"/>
+      <c r="D1035" s="1"/>
+      <c r="E1035" s="1"/>
+      <c r="F1035" s="1"/>
+      <c r="G1035" s="1"/>
+      <c r="H1035" s="1"/>
+      <c r="I1035" s="1"/>
+      <c r="J1035" s="1"/>
+      <c r="K1035" s="1"/>
+      <c r="L1035" s="1"/>
+      <c r="M1035" s="1"/>
+      <c r="N1035" s="1"/>
+      <c r="O1035" s="1"/>
+      <c r="P1035" s="1"/>
+      <c r="Q1035" s="1"/>
+      <c r="R1035" s="1"/>
+    </row>
+    <row r="1036" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1036" s="1"/>
+      <c r="B1036" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="1037" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1037">
+      <c r="C1036" s="1"/>
+      <c r="D1036" s="1"/>
+      <c r="E1036" s="1"/>
+      <c r="F1036" s="1"/>
+      <c r="G1036" s="1"/>
+      <c r="H1036" s="1"/>
+      <c r="I1036" s="1"/>
+      <c r="J1036" s="1"/>
+      <c r="K1036" s="1"/>
+      <c r="L1036" s="1"/>
+      <c r="M1036" s="1"/>
+      <c r="N1036" s="1"/>
+      <c r="O1036" s="1"/>
+      <c r="P1036" s="1"/>
+      <c r="Q1036" s="1"/>
+      <c r="R1036" s="1"/>
+    </row>
+    <row r="1037" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1037" s="1"/>
+      <c r="B1037" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="1038" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1038">
+      <c r="C1037" s="1"/>
+      <c r="D1037" s="1"/>
+      <c r="E1037" s="1"/>
+      <c r="F1037" s="1"/>
+      <c r="G1037" s="1"/>
+      <c r="H1037" s="1"/>
+      <c r="I1037" s="1"/>
+      <c r="J1037" s="1"/>
+      <c r="K1037" s="1"/>
+      <c r="L1037" s="1"/>
+      <c r="M1037" s="1"/>
+      <c r="N1037" s="1"/>
+      <c r="O1037" s="1"/>
+      <c r="P1037" s="1"/>
+      <c r="Q1037" s="1"/>
+      <c r="R1037" s="1"/>
+    </row>
+    <row r="1038" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1038" s="1"/>
+      <c r="B1038" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="1039" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1039" t="s">
+      <c r="C1038" s="1"/>
+      <c r="D1038" s="1"/>
+      <c r="E1038" s="1"/>
+      <c r="F1038" s="1"/>
+      <c r="G1038" s="1"/>
+      <c r="H1038" s="1"/>
+      <c r="I1038" s="1"/>
+      <c r="J1038" s="1"/>
+      <c r="K1038" s="1"/>
+      <c r="L1038" s="1"/>
+      <c r="M1038" s="1"/>
+      <c r="N1038" s="1"/>
+      <c r="O1038" s="1"/>
+      <c r="P1038" s="1"/>
+      <c r="Q1038" s="1"/>
+      <c r="R1038" s="1"/>
+    </row>
+    <row r="1039" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1039" s="1"/>
+      <c r="B1039" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="C1039" s="1"/>
+      <c r="D1039" s="1"/>
+      <c r="E1039" s="1"/>
+      <c r="F1039" s="1"/>
+      <c r="G1039" s="1"/>
+      <c r="H1039" s="1"/>
+      <c r="I1039" s="1"/>
+      <c r="J1039" s="1"/>
+      <c r="K1039" s="1"/>
+      <c r="L1039" s="1"/>
+      <c r="M1039" s="1"/>
+      <c r="N1039" s="1"/>
+      <c r="O1039" s="1"/>
+      <c r="P1039" s="1"/>
+      <c r="Q1039" s="1"/>
+      <c r="R1039" s="1"/>
+    </row>
+    <row r="1040" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1040" s="1"/>
+      <c r="B1040" s="1"/>
+      <c r="C1040" s="1"/>
+      <c r="D1040" s="1"/>
+      <c r="E1040" s="1"/>
+      <c r="F1040" s="1"/>
+      <c r="G1040" s="1"/>
+      <c r="H1040" s="1"/>
+      <c r="I1040" s="1"/>
+      <c r="J1040" s="1"/>
+      <c r="K1040" s="1"/>
+      <c r="L1040" s="1"/>
+      <c r="M1040" s="1"/>
+      <c r="N1040" s="1"/>
+      <c r="O1040" s="1"/>
+      <c r="P1040" s="1"/>
+      <c r="Q1040" s="1"/>
+      <c r="R1040" s="1"/>
+    </row>
+    <row r="1041" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1041" s="1"/>
+      <c r="B1041" s="1"/>
+      <c r="C1041" s="1"/>
+      <c r="D1041" s="1"/>
+      <c r="E1041" s="1"/>
+      <c r="F1041" s="1"/>
+      <c r="G1041" s="1"/>
+      <c r="H1041" s="1"/>
+      <c r="I1041" s="1"/>
+      <c r="J1041" s="1"/>
+      <c r="K1041" s="1"/>
+      <c r="L1041" s="1"/>
+      <c r="M1041" s="1"/>
+      <c r="N1041" s="1"/>
+      <c r="O1041" s="1"/>
+      <c r="P1041" s="1"/>
+      <c r="Q1041" s="1"/>
+      <c r="R1041" s="1"/>
+    </row>
+    <row r="1042" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1042" s="1"/>
+      <c r="B1042" s="1"/>
+      <c r="C1042" s="1"/>
+      <c r="D1042" s="1"/>
+      <c r="E1042" s="1"/>
+      <c r="F1042" s="1"/>
+      <c r="G1042" s="1"/>
+      <c r="H1042" s="1"/>
+      <c r="I1042" s="1"/>
+      <c r="J1042" s="1"/>
+      <c r="K1042" s="1"/>
+      <c r="L1042" s="1"/>
+      <c r="M1042" s="1"/>
+      <c r="N1042" s="1"/>
+      <c r="O1042" s="1"/>
+      <c r="P1042" s="1"/>
+      <c r="Q1042" s="1"/>
+      <c r="R1042" s="1"/>
     </row>
     <row r="1043" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1043" t="s">
+      <c r="A1043" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B1043" s="1"/>
+      <c r="C1043" s="1"/>
+      <c r="D1043" s="1"/>
+      <c r="E1043" s="1"/>
+      <c r="F1043" s="1"/>
+      <c r="G1043" s="1"/>
+      <c r="H1043" s="1"/>
+      <c r="I1043" s="1"/>
+      <c r="J1043" s="1"/>
+      <c r="K1043" s="1"/>
+      <c r="L1043" s="1"/>
+      <c r="M1043" s="1"/>
+      <c r="N1043" s="1"/>
+      <c r="O1043" s="1"/>
+      <c r="P1043" s="1"/>
+      <c r="Q1043" s="1"/>
+      <c r="R1043" s="1"/>
+    </row>
+    <row r="1044" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1044" s="1"/>
+      <c r="B1044" s="1"/>
+      <c r="C1044" s="1"/>
+      <c r="D1044" s="1"/>
+      <c r="E1044" s="1"/>
+      <c r="F1044" s="1"/>
+      <c r="G1044" s="1"/>
+      <c r="H1044" s="1"/>
+      <c r="I1044" s="1"/>
+      <c r="J1044" s="1"/>
+      <c r="K1044" s="1"/>
+      <c r="L1044" s="1"/>
+      <c r="M1044" s="1"/>
+      <c r="N1044" s="1"/>
+      <c r="O1044" s="1"/>
+      <c r="P1044" s="1"/>
+      <c r="Q1044" s="1"/>
+      <c r="R1044" s="1"/>
     </row>
     <row r="1045" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1045" s="1" t="s">
+      <c r="A1045" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="B1045" s="1"/>
+      <c r="C1045" s="1"/>
+      <c r="D1045" s="1"/>
+      <c r="E1045" s="1"/>
+      <c r="F1045" s="1"/>
+      <c r="G1045" s="1"/>
+      <c r="H1045" s="1"/>
+      <c r="I1045" s="1"/>
+      <c r="J1045" s="1"/>
+      <c r="K1045" s="1"/>
+      <c r="L1045" s="1"/>
+      <c r="M1045" s="1"/>
+      <c r="N1045" s="1"/>
+      <c r="O1045" s="1"/>
+      <c r="P1045" s="1"/>
+      <c r="Q1045" s="1"/>
+      <c r="R1045" s="1"/>
     </row>
     <row r="1046" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1046" s="2" t="s">
+      <c r="A1046" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B1046" s="2"/>
-      <c r="C1046" s="2"/>
-      <c r="D1046" s="2"/>
-      <c r="E1046" s="2"/>
-      <c r="G1046" s="2" t="s">
+      <c r="B1046" s="4"/>
+      <c r="C1046" s="4"/>
+      <c r="D1046" s="4"/>
+      <c r="E1046" s="4"/>
+      <c r="F1046" s="1"/>
+      <c r="G1046" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H1046" s="2"/>
-      <c r="I1046" s="2"/>
-      <c r="J1046" s="2"/>
-      <c r="K1046" s="2"/>
-      <c r="L1046" s="2"/>
-      <c r="N1046" s="3" t="s">
+      <c r="H1046" s="4"/>
+      <c r="I1046" s="4"/>
+      <c r="J1046" s="4"/>
+      <c r="K1046" s="4"/>
+      <c r="L1046" s="4"/>
+      <c r="M1046" s="1"/>
+      <c r="N1046" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O1046" s="2"/>
-      <c r="P1046" s="2"/>
-      <c r="Q1046" s="2"/>
-      <c r="R1046" s="2"/>
+      <c r="O1046" s="4"/>
+      <c r="P1046" s="4"/>
+      <c r="Q1046" s="4"/>
+      <c r="R1046" s="4"/>
     </row>
     <row r="1047" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1047" s="2" t="s">
+      <c r="A1047" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1047" s="2"/>
-      <c r="C1047" s="2"/>
-      <c r="D1047" s="2"/>
-      <c r="E1047" s="2"/>
-      <c r="G1047" s="2" t="s">
+      <c r="B1047" s="4"/>
+      <c r="C1047" s="4"/>
+      <c r="D1047" s="4"/>
+      <c r="E1047" s="4"/>
+      <c r="F1047" s="1"/>
+      <c r="G1047" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H1047" s="2"/>
-      <c r="I1047" s="2"/>
-      <c r="J1047" s="2"/>
-      <c r="K1047" s="2"/>
-      <c r="L1047" s="2"/>
-      <c r="N1047" s="3" t="s">
+      <c r="H1047" s="4"/>
+      <c r="I1047" s="4"/>
+      <c r="J1047" s="4"/>
+      <c r="K1047" s="4"/>
+      <c r="L1047" s="4"/>
+      <c r="M1047" s="1"/>
+      <c r="N1047" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O1047" s="2"/>
-      <c r="P1047" s="2"/>
-      <c r="Q1047" s="2"/>
-      <c r="R1047" s="2"/>
+      <c r="O1047" s="4"/>
+      <c r="P1047" s="4"/>
+      <c r="Q1047" s="4"/>
+      <c r="R1047" s="4"/>
     </row>
     <row r="1048" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1048" s="2" t="s">
+      <c r="A1048" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B1048" s="2"/>
-      <c r="C1048" s="2"/>
-      <c r="D1048" s="2"/>
-      <c r="E1048" s="2"/>
-      <c r="G1048" s="2" t="s">
+      <c r="B1048" s="4"/>
+      <c r="C1048" s="4"/>
+      <c r="D1048" s="4"/>
+      <c r="E1048" s="4"/>
+      <c r="F1048" s="1"/>
+      <c r="G1048" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H1048" s="2"/>
-      <c r="I1048" s="2"/>
-      <c r="J1048" s="2"/>
-      <c r="K1048" s="2"/>
-      <c r="L1048" s="2"/>
-      <c r="N1048" s="2" t="s">
+      <c r="H1048" s="4"/>
+      <c r="I1048" s="4"/>
+      <c r="J1048" s="4"/>
+      <c r="K1048" s="4"/>
+      <c r="L1048" s="4"/>
+      <c r="M1048" s="1"/>
+      <c r="N1048" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O1048" s="2"/>
-      <c r="P1048" s="2"/>
-      <c r="Q1048" s="2"/>
-      <c r="R1048" s="2"/>
+      <c r="O1048" s="4"/>
+      <c r="P1048" s="4"/>
+      <c r="Q1048" s="4"/>
+      <c r="R1048" s="4"/>
     </row>
     <row r="1049" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1049" s="2" t="s">
+      <c r="A1049" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B1049" s="2"/>
-      <c r="C1049" s="2"/>
-      <c r="D1049" s="2"/>
-      <c r="E1049" s="2"/>
-      <c r="G1049" s="2" t="s">
+      <c r="B1049" s="4"/>
+      <c r="C1049" s="4"/>
+      <c r="D1049" s="4"/>
+      <c r="E1049" s="4"/>
+      <c r="F1049" s="1"/>
+      <c r="G1049" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H1049" s="2"/>
-      <c r="I1049" s="2"/>
-      <c r="J1049" s="2"/>
-      <c r="K1049" s="2"/>
-      <c r="L1049" s="2"/>
-      <c r="N1049" s="1" t="s">
+      <c r="H1049" s="4"/>
+      <c r="I1049" s="4"/>
+      <c r="J1049" s="4"/>
+      <c r="K1049" s="4"/>
+      <c r="L1049" s="4"/>
+      <c r="M1049" s="1"/>
+      <c r="N1049" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="O1049" s="1"/>
+      <c r="P1049" s="1"/>
+      <c r="Q1049" s="1"/>
+      <c r="R1049" s="1"/>
     </row>
     <row r="1050" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1050" s="2" t="s">
+      <c r="A1050" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1050" s="2"/>
-      <c r="C1050" s="2"/>
-      <c r="D1050" s="2"/>
-      <c r="E1050" s="2"/>
-      <c r="G1050" s="2" t="s">
+      <c r="B1050" s="4"/>
+      <c r="C1050" s="4"/>
+      <c r="D1050" s="4"/>
+      <c r="E1050" s="4"/>
+      <c r="F1050" s="1"/>
+      <c r="G1050" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H1050" s="2"/>
-      <c r="I1050" s="2"/>
-      <c r="J1050" s="2"/>
-      <c r="K1050" s="2"/>
-      <c r="L1050" s="2"/>
+      <c r="H1050" s="4"/>
+      <c r="I1050" s="4"/>
+      <c r="J1050" s="4"/>
+      <c r="K1050" s="4"/>
+      <c r="L1050" s="4"/>
+      <c r="M1050" s="1"/>
+      <c r="N1050" s="1"/>
+      <c r="O1050" s="1"/>
+      <c r="P1050" s="1"/>
+      <c r="Q1050" s="1"/>
+      <c r="R1050" s="1"/>
     </row>
     <row r="1051" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1051" s="2" t="s">
+      <c r="A1051" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B1051" s="2"/>
-      <c r="C1051" s="2"/>
-      <c r="D1051" s="2"/>
-      <c r="E1051" s="2"/>
-      <c r="G1051" s="3" t="s">
+      <c r="B1051" s="4"/>
+      <c r="C1051" s="4"/>
+      <c r="D1051" s="4"/>
+      <c r="E1051" s="4"/>
+      <c r="F1051" s="1"/>
+      <c r="G1051" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H1051" s="2"/>
-      <c r="I1051" s="2"/>
-      <c r="J1051" s="2"/>
-      <c r="K1051" s="2"/>
-      <c r="L1051" s="2"/>
+      <c r="H1051" s="4"/>
+      <c r="I1051" s="4"/>
+      <c r="J1051" s="4"/>
+      <c r="K1051" s="4"/>
+      <c r="L1051" s="4"/>
+      <c r="M1051" s="1"/>
+      <c r="N1051" s="1"/>
+      <c r="O1051" s="1"/>
+      <c r="P1051" s="1"/>
+      <c r="Q1051" s="1"/>
+      <c r="R1051" s="1"/>
     </row>
     <row r="1052" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1052" s="2" t="s">
+      <c r="A1052" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B1052" s="2"/>
-      <c r="C1052" s="2"/>
-      <c r="D1052" s="2"/>
-      <c r="E1052" s="2"/>
-      <c r="G1052" s="3" t="s">
+      <c r="B1052" s="4"/>
+      <c r="C1052" s="4"/>
+      <c r="D1052" s="4"/>
+      <c r="E1052" s="4"/>
+      <c r="F1052" s="1"/>
+      <c r="G1052" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H1052" s="2"/>
-      <c r="I1052" s="2"/>
-      <c r="J1052" s="2"/>
-      <c r="K1052" s="2"/>
-      <c r="L1052" s="2"/>
+      <c r="H1052" s="4"/>
+      <c r="I1052" s="4"/>
+      <c r="J1052" s="4"/>
+      <c r="K1052" s="4"/>
+      <c r="L1052" s="4"/>
+      <c r="M1052" s="1"/>
+      <c r="N1052" s="1"/>
+      <c r="O1052" s="1"/>
+      <c r="P1052" s="1"/>
+      <c r="Q1052" s="1"/>
+      <c r="R1052" s="1"/>
     </row>
     <row r="1053" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1053" s="2" t="s">
+      <c r="A1053" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B1053" s="2"/>
-      <c r="C1053" s="2"/>
-      <c r="D1053" s="2"/>
-      <c r="E1053" s="2"/>
-      <c r="G1053" s="3" t="s">
+      <c r="B1053" s="4"/>
+      <c r="C1053" s="4"/>
+      <c r="D1053" s="4"/>
+      <c r="E1053" s="4"/>
+      <c r="F1053" s="1"/>
+      <c r="G1053" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H1053" s="2"/>
-      <c r="I1053" s="2"/>
-      <c r="J1053" s="2"/>
-      <c r="K1053" s="2"/>
-      <c r="L1053" s="2"/>
+      <c r="H1053" s="4"/>
+      <c r="I1053" s="4"/>
+      <c r="J1053" s="4"/>
+      <c r="K1053" s="4"/>
+      <c r="L1053" s="4"/>
+      <c r="M1053" s="1"/>
+      <c r="N1053" s="1"/>
+      <c r="O1053" s="1"/>
+      <c r="P1053" s="1"/>
+      <c r="Q1053" s="1"/>
+      <c r="R1053" s="1"/>
     </row>
     <row r="1054" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1054" s="2" t="s">
+      <c r="A1054" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B1054" s="2"/>
-      <c r="C1054" s="2"/>
-      <c r="D1054" s="2"/>
-      <c r="E1054" s="2"/>
-      <c r="G1054" s="2" t="s">
+      <c r="B1054" s="4"/>
+      <c r="C1054" s="4"/>
+      <c r="D1054" s="4"/>
+      <c r="E1054" s="4"/>
+      <c r="F1054" s="1"/>
+      <c r="G1054" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H1054" s="2"/>
-      <c r="I1054" s="2"/>
-      <c r="J1054" s="2"/>
-      <c r="K1054" s="2"/>
-      <c r="L1054" s="2"/>
+      <c r="H1054" s="4"/>
+      <c r="I1054" s="4"/>
+      <c r="J1054" s="4"/>
+      <c r="K1054" s="4"/>
+      <c r="L1054" s="4"/>
+      <c r="M1054" s="1"/>
+      <c r="N1054" s="1"/>
+      <c r="O1054" s="1"/>
+      <c r="P1054" s="1"/>
+      <c r="Q1054" s="1"/>
+      <c r="R1054" s="1"/>
+    </row>
+    <row r="1055" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1055" s="1"/>
+      <c r="B1055" s="1"/>
+      <c r="C1055" s="1"/>
+      <c r="D1055" s="1"/>
+      <c r="E1055" s="1"/>
+      <c r="F1055" s="1"/>
+      <c r="G1055" s="1"/>
+      <c r="H1055" s="1"/>
+      <c r="I1055" s="1"/>
+      <c r="J1055" s="1"/>
+      <c r="K1055" s="1"/>
+      <c r="L1055" s="1"/>
+      <c r="M1055" s="1"/>
+      <c r="N1055" s="1"/>
+      <c r="O1055" s="1"/>
+      <c r="P1055" s="1"/>
+      <c r="Q1055" s="1"/>
+      <c r="R1055" s="1"/>
+    </row>
+    <row r="1056" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1056" s="1"/>
+      <c r="B1056" s="1"/>
+      <c r="C1056" s="1"/>
+      <c r="D1056" s="1"/>
+      <c r="E1056" s="1"/>
+      <c r="F1056" s="1"/>
+      <c r="G1056" s="1"/>
+      <c r="H1056" s="1"/>
+      <c r="I1056" s="1"/>
+      <c r="J1056" s="1"/>
+      <c r="K1056" s="1"/>
+      <c r="L1056" s="1"/>
+      <c r="M1056" s="1"/>
+      <c r="N1056" s="1"/>
+      <c r="O1056" s="1"/>
+      <c r="P1056" s="1"/>
+      <c r="Q1056" s="1"/>
+      <c r="R1056" s="1"/>
     </row>
     <row r="1057" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1057" t="s">
+      <c r="A1057" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="B1057" s="1"/>
+      <c r="C1057" s="1"/>
+      <c r="D1057" s="1"/>
+      <c r="E1057" s="1"/>
+      <c r="F1057" s="1"/>
+      <c r="G1057" s="1"/>
+      <c r="H1057" s="1"/>
+      <c r="I1057" s="1"/>
+      <c r="J1057" s="1"/>
+      <c r="K1057" s="1"/>
+      <c r="L1057" s="1"/>
+      <c r="M1057" s="1"/>
+      <c r="N1057" s="1"/>
+      <c r="O1057" s="1"/>
+      <c r="P1057" s="1"/>
+      <c r="Q1057" s="1"/>
+      <c r="R1057" s="1"/>
     </row>
     <row r="1058" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1058" s="2" t="s">
+      <c r="A1058" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B1058" s="2"/>
-      <c r="C1058" s="2"/>
-      <c r="D1058" s="2"/>
-      <c r="E1058" s="2"/>
-      <c r="G1058" s="2" t="s">
+      <c r="B1058" s="4"/>
+      <c r="C1058" s="4"/>
+      <c r="D1058" s="4"/>
+      <c r="E1058" s="4"/>
+      <c r="F1058" s="1"/>
+      <c r="G1058" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H1058" s="2"/>
-      <c r="I1058" s="2"/>
-      <c r="J1058" s="2"/>
-      <c r="K1058" s="2"/>
-      <c r="L1058" s="2"/>
-      <c r="N1058" s="2" t="s">
+      <c r="H1058" s="4"/>
+      <c r="I1058" s="4"/>
+      <c r="J1058" s="4"/>
+      <c r="K1058" s="4"/>
+      <c r="L1058" s="4"/>
+      <c r="M1058" s="1"/>
+      <c r="N1058" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="O1058" s="2"/>
-      <c r="P1058" s="2"/>
-      <c r="Q1058" s="2"/>
-      <c r="R1058" s="2"/>
+      <c r="O1058" s="4"/>
+      <c r="P1058" s="4"/>
+      <c r="Q1058" s="4"/>
+      <c r="R1058" s="4"/>
     </row>
     <row r="1059" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1059" s="2" t="s">
+      <c r="A1059" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1059" s="2"/>
-      <c r="C1059" s="2"/>
-      <c r="D1059" s="2"/>
-      <c r="E1059" s="2"/>
-      <c r="G1059" s="2" t="s">
+      <c r="B1059" s="4"/>
+      <c r="C1059" s="4"/>
+      <c r="D1059" s="4"/>
+      <c r="E1059" s="4"/>
+      <c r="F1059" s="1"/>
+      <c r="G1059" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H1059" s="2"/>
-      <c r="I1059" s="2"/>
-      <c r="J1059" s="2"/>
-      <c r="K1059" s="2"/>
-      <c r="L1059" s="2"/>
-      <c r="N1059" s="2" t="s">
+      <c r="H1059" s="4"/>
+      <c r="I1059" s="4"/>
+      <c r="J1059" s="4"/>
+      <c r="K1059" s="4"/>
+      <c r="L1059" s="4"/>
+      <c r="M1059" s="1"/>
+      <c r="N1059" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="O1059" s="2"/>
-      <c r="P1059" s="2"/>
-      <c r="Q1059" s="2"/>
-      <c r="R1059" s="2"/>
+      <c r="O1059" s="4"/>
+      <c r="P1059" s="4"/>
+      <c r="Q1059" s="4"/>
+      <c r="R1059" s="4"/>
     </row>
     <row r="1060" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1060" s="2" t="s">
+      <c r="A1060" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1060" s="2"/>
-      <c r="C1060" s="2"/>
-      <c r="D1060" s="2"/>
-      <c r="E1060" s="2"/>
-      <c r="G1060" s="2" t="s">
+      <c r="B1060" s="4"/>
+      <c r="C1060" s="4"/>
+      <c r="D1060" s="4"/>
+      <c r="E1060" s="4"/>
+      <c r="F1060" s="1"/>
+      <c r="G1060" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H1060" s="2"/>
-      <c r="I1060" s="2"/>
-      <c r="J1060" s="2"/>
-      <c r="K1060" s="2"/>
-      <c r="L1060" s="2"/>
-      <c r="N1060" s="2" t="s">
+      <c r="H1060" s="4"/>
+      <c r="I1060" s="4"/>
+      <c r="J1060" s="4"/>
+      <c r="K1060" s="4"/>
+      <c r="L1060" s="4"/>
+      <c r="M1060" s="1"/>
+      <c r="N1060" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="O1060" s="2"/>
-      <c r="P1060" s="2"/>
-      <c r="Q1060" s="2"/>
-      <c r="R1060" s="2"/>
+      <c r="O1060" s="4"/>
+      <c r="P1060" s="4"/>
+      <c r="Q1060" s="4"/>
+      <c r="R1060" s="4"/>
     </row>
     <row r="1061" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1061" s="2" t="s">
+      <c r="A1061" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B1061" s="2"/>
-      <c r="C1061" s="2"/>
-      <c r="D1061" s="2"/>
-      <c r="E1061" s="2"/>
-      <c r="G1061" s="2" t="s">
+      <c r="B1061" s="4"/>
+      <c r="C1061" s="4"/>
+      <c r="D1061" s="4"/>
+      <c r="E1061" s="4"/>
+      <c r="F1061" s="1"/>
+      <c r="G1061" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H1061" s="2"/>
-      <c r="I1061" s="2"/>
-      <c r="J1061" s="2"/>
-      <c r="K1061" s="2"/>
-      <c r="L1061" s="2"/>
+      <c r="H1061" s="4"/>
+      <c r="I1061" s="4"/>
+      <c r="J1061" s="4"/>
+      <c r="K1061" s="4"/>
+      <c r="L1061" s="4"/>
+      <c r="M1061" s="1"/>
+      <c r="N1061" s="1"/>
+      <c r="O1061" s="1"/>
+      <c r="P1061" s="1"/>
+      <c r="Q1061" s="1"/>
+      <c r="R1061" s="1"/>
     </row>
     <row r="1062" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1062" s="2" t="s">
+      <c r="A1062" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B1062" s="2"/>
-      <c r="C1062" s="2"/>
-      <c r="D1062" s="2"/>
-      <c r="E1062" s="2"/>
-      <c r="G1062" s="2" t="s">
+      <c r="B1062" s="4"/>
+      <c r="C1062" s="4"/>
+      <c r="D1062" s="4"/>
+      <c r="E1062" s="4"/>
+      <c r="F1062" s="1"/>
+      <c r="G1062" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H1062" s="2"/>
-      <c r="I1062" s="2"/>
-      <c r="J1062" s="2"/>
-      <c r="K1062" s="2"/>
-      <c r="L1062" s="2"/>
+      <c r="H1062" s="4"/>
+      <c r="I1062" s="4"/>
+      <c r="J1062" s="4"/>
+      <c r="K1062" s="4"/>
+      <c r="L1062" s="4"/>
+      <c r="M1062" s="1"/>
+      <c r="N1062" s="1"/>
+      <c r="O1062" s="1"/>
+      <c r="P1062" s="1"/>
+      <c r="Q1062" s="1"/>
+      <c r="R1062" s="1"/>
     </row>
     <row r="1063" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1063" s="2" t="s">
+      <c r="A1063" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B1063" s="2"/>
-      <c r="C1063" s="2"/>
-      <c r="D1063" s="2"/>
-      <c r="E1063" s="2"/>
-      <c r="G1063" s="2" t="s">
+      <c r="B1063" s="4"/>
+      <c r="C1063" s="4"/>
+      <c r="D1063" s="4"/>
+      <c r="E1063" s="4"/>
+      <c r="F1063" s="1"/>
+      <c r="G1063" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H1063" s="2"/>
-      <c r="I1063" s="2"/>
-      <c r="J1063" s="2"/>
-      <c r="K1063" s="2"/>
-      <c r="L1063" s="2"/>
+      <c r="H1063" s="4"/>
+      <c r="I1063" s="4"/>
+      <c r="J1063" s="4"/>
+      <c r="K1063" s="4"/>
+      <c r="L1063" s="4"/>
+      <c r="M1063" s="1"/>
+      <c r="N1063" s="1"/>
+      <c r="O1063" s="1"/>
+      <c r="P1063" s="1"/>
+      <c r="Q1063" s="1"/>
+      <c r="R1063" s="1"/>
     </row>
     <row r="1064" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1064" s="2" t="s">
+      <c r="A1064" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B1064" s="2"/>
-      <c r="C1064" s="2"/>
-      <c r="D1064" s="2"/>
-      <c r="E1064" s="2"/>
-      <c r="G1064" s="2" t="s">
+      <c r="B1064" s="4"/>
+      <c r="C1064" s="4"/>
+      <c r="D1064" s="4"/>
+      <c r="E1064" s="4"/>
+      <c r="F1064" s="1"/>
+      <c r="G1064" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H1064" s="2"/>
-      <c r="I1064" s="2"/>
-      <c r="J1064" s="2"/>
-      <c r="K1064" s="2"/>
-      <c r="L1064" s="2"/>
+      <c r="H1064" s="4"/>
+      <c r="I1064" s="4"/>
+      <c r="J1064" s="4"/>
+      <c r="K1064" s="4"/>
+      <c r="L1064" s="4"/>
+      <c r="M1064" s="1"/>
+      <c r="N1064" s="1"/>
+      <c r="O1064" s="1"/>
+      <c r="P1064" s="1"/>
+      <c r="Q1064" s="1"/>
+      <c r="R1064" s="1"/>
     </row>
     <row r="1065" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1065" s="2" t="s">
+      <c r="A1065" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B1065" s="2"/>
-      <c r="C1065" s="2"/>
-      <c r="D1065" s="2"/>
-      <c r="E1065" s="2"/>
-      <c r="G1065" s="2" t="s">
+      <c r="B1065" s="4"/>
+      <c r="C1065" s="4"/>
+      <c r="D1065" s="4"/>
+      <c r="E1065" s="4"/>
+      <c r="F1065" s="1"/>
+      <c r="G1065" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H1065" s="2"/>
-      <c r="I1065" s="2"/>
-      <c r="J1065" s="2"/>
-      <c r="K1065" s="2"/>
-      <c r="L1065" s="2"/>
+      <c r="H1065" s="4"/>
+      <c r="I1065" s="4"/>
+      <c r="J1065" s="4"/>
+      <c r="K1065" s="4"/>
+      <c r="L1065" s="4"/>
+      <c r="M1065" s="1"/>
+      <c r="N1065" s="1"/>
+      <c r="O1065" s="1"/>
+      <c r="P1065" s="1"/>
+      <c r="Q1065" s="1"/>
+      <c r="R1065" s="1"/>
     </row>
     <row r="1066" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1066" s="2" t="s">
+      <c r="A1066" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B1066" s="2"/>
-      <c r="C1066" s="2"/>
-      <c r="D1066" s="2"/>
-      <c r="E1066" s="2"/>
-      <c r="G1066" s="2" t="s">
+      <c r="B1066" s="4"/>
+      <c r="C1066" s="4"/>
+      <c r="D1066" s="4"/>
+      <c r="E1066" s="4"/>
+      <c r="F1066" s="1"/>
+      <c r="G1066" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H1066" s="2"/>
-      <c r="I1066" s="2"/>
-      <c r="J1066" s="2"/>
-      <c r="K1066" s="2"/>
-      <c r="L1066" s="2"/>
+      <c r="H1066" s="4"/>
+      <c r="I1066" s="4"/>
+      <c r="J1066" s="4"/>
+      <c r="K1066" s="4"/>
+      <c r="L1066" s="4"/>
+      <c r="M1066" s="1"/>
+      <c r="N1066" s="1"/>
+      <c r="O1066" s="1"/>
+      <c r="P1066" s="1"/>
+      <c r="Q1066" s="1"/>
+      <c r="R1066" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="42">

</xml_diff>